<commit_message>
Se actualiso el calendario pero con algunos errores para arreglar
</commit_message>
<xml_diff>
--- a/staticfiles/templates/plantilla_instructores.xlsx
+++ b/staticfiles/templates/plantilla_instructores.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,9 +456,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="37" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
@@ -493,27 +493,405 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Juan Carlos</t>
+          <t>Jesus Andres</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pérez González</t>
+          <t>Silva Plazas</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>jperez@sena.edu.co</t>
+          <t>jsapp@sena.edu.co</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3001234567</t>
+          <t>3148777918</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1234567890</t>
+          <t>1077848000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sebastian</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ramirez Rojas</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sebastian_ramirezro@soy.sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3133516648</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1077848001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ramirez</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3118777918</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1077488000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rodriguez</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3157894562</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1082654789</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3209876543</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1098765432</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ana</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Martinez</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3112345678</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1045678912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Lopez</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3145678901</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1034567890</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Patricia</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3187654321</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1067891234</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hernandez</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3198765432</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1056789123</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Laura</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Sanchez</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3167891234</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1023456789</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Miguel</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Torres</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3178912345</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1012345678</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Carmen</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Perez</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3123456789</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1089123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ricardo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Diaz</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3134567890</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1078912345</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Valeria</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Jimenez</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3190123456</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1001234567</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Reyes</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>joseramirez@sena.edu.co</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3212345678</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1087654321</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Eliminar imágenes placeholder y limpieza de código
</commit_message>
<xml_diff>
--- a/staticfiles/templates/plantilla_instructores.xlsx
+++ b/staticfiles/templates/plantilla_instructores.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,8 +457,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
@@ -493,351 +493,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jesus Andres</t>
+          <t>Juan Carlos</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Silva Plazas</t>
+          <t>Pérez González</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>jsapp@sena.edu.co</t>
+          <t>jperez@sena.edu.co</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3148777918</t>
+          <t>3001234567</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1077848000</t>
+          <t>1234567890</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>Jesus Andres</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ramirez</t>
+          <t>Silva Plazas</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>joseramirez@sena.edu.co</t>
+          <t>jsapp@sena.edu.co</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3118777918</t>
+          <t>3182528515</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1077488000</t>
+          <t>1055878001</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>Jesurum Rojas</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>joseramirez@sena.edu.co</t>
+          <t>gabrieljesurumro@sena.edu.co</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3157894562</t>
+          <t>3143887918</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1082654789</t>
+          <t>3125435</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Carlos</t>
+          <t>Hector</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Plaz Plaza</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>joseramirez@sena.edu.co</t>
+          <t>hector@sena.edu.co</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3209876543</t>
+          <t>3142884050</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1098765432</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Ana</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Martinez</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3112345678</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1045678912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Juan</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Lopez</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>3145678901</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1034567890</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Patricia</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Gomez</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>3187654321</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1067891234</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Diego</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Hernandez</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>3198765432</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1056789123</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Laura</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Sanchez</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>3167891234</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1023456789</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Miguel</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Torres</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>3178912345</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1012345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Carmen</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Perez</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>3123456789</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1089123456</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Ricardo</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Diaz</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>3134567890</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1078912345</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Carolina</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Reyes</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>joseramirez@sena.edu.co</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>3212345678</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1087654321</t>
+          <t>107784658</t>
         </is>
       </c>
     </row>

</xml_diff>